<commit_message>
Some files are left out
</commit_message>
<xml_diff>
--- a/Resources/Project Reference/090259.xlsx
+++ b/Resources/Project Reference/090259.xlsx
@@ -1152,8 +1152,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F05C1EF0044CF249A09568BFC7A27DEF" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7bab7cd2411e049573f4a65da80024b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="360d23a6-f195-4c5c-b5bb-19aa4319b9ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aa57f365afa5b6f0db785387c52e466" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F05C1EF0044CF249A09568BFC7A27DEF" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a308155717e7f8eadebf0d848e17ba4f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="360d23a6-f195-4c5c-b5bb-19aa4319b9ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1d6afd8dd879a1d7a61ed4bc2f66470" ns2:_="">
     <xsd:import namespace="360d23a6-f195-4c5c-b5bb-19aa4319b9ef"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1163,6 +1163,9 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1181,6 +1184,23 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1299,7 +1319,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413060F-A3D2-48E6-B361-6969D3CA01F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F318854-E18F-49A4-9E12-60311B565E36}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Edit Micrsoft Flow thing
</commit_message>
<xml_diff>
--- a/Resources/Project Reference/090259.xlsx
+++ b/Resources/Project Reference/090259.xlsx
@@ -1152,8 +1152,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F05C1EF0044CF249A09568BFC7A27DEF" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7bab7cd2411e049573f4a65da80024b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="360d23a6-f195-4c5c-b5bb-19aa4319b9ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aa57f365afa5b6f0db785387c52e466" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F05C1EF0044CF249A09568BFC7A27DEF" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a308155717e7f8eadebf0d848e17ba4f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="360d23a6-f195-4c5c-b5bb-19aa4319b9ef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1d6afd8dd879a1d7a61ed4bc2f66470" ns2:_="">
     <xsd:import namespace="360d23a6-f195-4c5c-b5bb-19aa4319b9ef"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1163,6 +1163,9 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1181,6 +1184,23 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1299,7 +1319,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413060F-A3D2-48E6-B361-6969D3CA01F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F318854-E18F-49A4-9E12-60311B565E36}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>